<commit_message>
add 3 groups of data hyy hzj cxq
</commit_message>
<xml_diff>
--- a/Data/全部数据/原始excel/调节6Hz(K=1~2)/k=1.0/k=1.0所有概率值.xlsx
+++ b/Data/全部数据/原始excel/调节6Hz(K=1~2)/k=1.0/k=1.0所有概率值.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="11655"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13170"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>lz-调节6hz_20170106_105432_ASIC_EEG</t>
   </si>
@@ -36,6 +36,15 @@
   </si>
   <si>
     <t>wnb-调节6Hz_20170110_113300_ASIC_EEG</t>
+  </si>
+  <si>
+    <t>cxq6hz_20170224_144343_ASIC_EEG</t>
+  </si>
+  <si>
+    <t>hyy-调节6Hz_20170306_110203_ASIC_EEG</t>
+  </si>
+  <si>
+    <t>hzj-调节6Hz_20170220_113105_ASIC_EEG</t>
   </si>
 </sst>
 </file>
@@ -365,15 +374,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D3"/>
+      <selection sqref="A1:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -386,8 +395,17 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0.67449664429530198</v>
       </c>
@@ -400,8 +418,17 @@
       <c r="D2">
         <v>0.49838187702265369</v>
       </c>
+      <c r="E2">
+        <v>0.5370919881305638</v>
+      </c>
+      <c r="F2">
+        <v>0.57575757575757569</v>
+      </c>
+      <c r="G2">
+        <v>0.53453453453453448</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0.7</v>
       </c>
@@ -413,6 +440,15 @@
       </c>
       <c r="D3">
         <v>0.70648464163822533</v>
+      </c>
+      <c r="E3">
+        <v>0.58309037900874627</v>
+      </c>
+      <c r="F3">
+        <v>0.60409556313993173</v>
+      </c>
+      <c r="G3">
+        <v>0.61612903225806459</v>
       </c>
     </row>
   </sheetData>

</xml_diff>